<commit_message>
Test successful with mock user data in Excel
</commit_message>
<xml_diff>
--- a/Data/mock_user_data.xlsx
+++ b/Data/mock_user_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatabandi/google_backup/test_automation/robot-test-automation-sauce-demo/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CC4F61-C1E8-D74E-B2F6-C29F16DB1F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37A6FDA-46C3-E64A-ABB3-F06E2EFD27B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{A13B7221-93B5-2A4F-82F3-AE689C8CC65A}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>standard_user</t>
   </si>
   <si>
@@ -62,7 +59,10 @@
     <t>secret_sauce</t>
   </si>
   <si>
-    <t>username</t>
+    <t>${username}</t>
+  </si>
+  <si>
+    <t>${password}</t>
   </si>
 </sst>
 </file>
@@ -436,9 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61461CD0-15D1-F04B-86FE-E70D99EB0507}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -447,58 +445,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing drop down menu functionality for item list on logedin page
</commit_message>
<xml_diff>
--- a/Data/mock_user_data.xlsx
+++ b/Data/mock_user_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatabandi/google_backup/test_automation/robot-test-automation-sauce-demo/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatabandi/google_backup/ta-sausedemo/ta-sausedemo/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37A6FDA-46C3-E64A-ABB3-F06E2EFD27B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B533ECDD-03B7-144D-84CC-9BBA280E6764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{A13B7221-93B5-2A4F-82F3-AE689C8CC65A}"/>
+    <workbookView xWindow="36500" yWindow="6200" windowWidth="28040" windowHeight="17440" xr2:uid="{A13B7221-93B5-2A4F-82F3-AE689C8CC65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>